<commit_message>
whoops needed another instruction to protect a value
</commit_message>
<xml_diff>
--- a/Excel_Binary/PseudoBinaryGuide.xlsx
+++ b/Excel_Binary/PseudoBinaryGuide.xlsx
@@ -1,41 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CompArch_2015\Excel_Binary\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="8505"/>
+    <workbookView xWindow="120" yWindow="80" windowWidth="9460" windowHeight="7840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
-  <si>
-    <t>addi $a1, $a1, -1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>lw $t0, Mem[$a0]</t>
   </si>
   <si>
-    <t>ble $t0, 80[hex], else</t>
-  </si>
-  <si>
     <t>srl $v0, $v0, 3</t>
   </si>
   <si>
     <t>or $v1, $v1, $v0</t>
   </si>
   <si>
-    <t>sw Mem[$a0], F0[hex]</t>
-  </si>
-  <si>
     <t>j post if</t>
   </si>
   <si>
@@ -51,9 +50,6 @@
     <t>xor $v3, $v3, $v2</t>
   </si>
   <si>
-    <t>sw Mem[$a0], 0F[hex]</t>
-  </si>
-  <si>
     <t>post if:</t>
   </si>
   <si>
@@ -69,9 +65,6 @@
     <t>1000 001 001 111111</t>
   </si>
   <si>
-    <t>1100 101 000 xxxxxx</t>
-  </si>
-  <si>
     <t>0001 101 110 xxxxxx</t>
   </si>
   <si>
@@ -81,29 +74,146 @@
     <t>1001 001 011 001 000</t>
   </si>
   <si>
-    <t>0000 xxxxxxxxxxxx</t>
-  </si>
-  <si>
-    <t>0010 001 000 xxxxxx</t>
-  </si>
-  <si>
     <t>1000 000 000 000010</t>
   </si>
   <si>
-    <t>1101 000 000 xxxxxx</t>
-  </si>
-  <si>
-    <t>1100 100 011 100 000</t>
-  </si>
-  <si>
     <t>1010 011 010 011 000</t>
+  </si>
+  <si>
+    <t>ble $t0, 0100[hex], else</t>
+  </si>
+  <si>
+    <t>RAW $t0</t>
+  </si>
+  <si>
+    <t>RAW $v0</t>
+  </si>
+  <si>
+    <t>RAW $v2</t>
+  </si>
+  <si>
+    <t>1100 101 000 000000</t>
+  </si>
+  <si>
+    <t>1101 xxx 000 000000</t>
+  </si>
+  <si>
+    <t>sw Mem[$a0], 00FF[hex]</t>
+  </si>
+  <si>
+    <t>0010 001 000 000001</t>
+  </si>
+  <si>
+    <t>0000 000 000 0001011</t>
+  </si>
+  <si>
+    <t>store 00FF[hex] in earlier instruction</t>
+  </si>
+  <si>
+    <t>sw temp, mem[$a0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sll $t0, $t0, </t>
+  </si>
+  <si>
+    <t>// store FF00[hex] early or 0000[hex] with 1111 1111 0000 0000</t>
+  </si>
+  <si>
+    <t>lw $t1, Mem[$a4]</t>
+  </si>
+  <si>
+    <t>lw $t2, Mem[$a5]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">or $t, $, </t>
+  </si>
+  <si>
+    <t>andi $a1, $a1, -1</t>
+  </si>
+  <si>
+    <t>lw $t1, Mem[$a1]</t>
+  </si>
+  <si>
+    <t>sw $t1, Mem[$a1]</t>
+  </si>
+  <si>
+    <t>addi $t1, $t1, -1</t>
+  </si>
+  <si>
+    <t>ble $t0, $t1, else</t>
+  </si>
+  <si>
+    <t>//if statement</t>
+  </si>
+  <si>
+    <t>lw $t2, Mem[$a4]</t>
+  </si>
+  <si>
+    <t>// else</t>
+  </si>
+  <si>
+    <t>sw $t2, Mem[$a0]</t>
+  </si>
+  <si>
+    <t>// post if</t>
+  </si>
+  <si>
+    <t>//top</t>
+  </si>
+  <si>
+    <t>//return</t>
+  </si>
+  <si>
+    <t>addi $t0, $t0, 2</t>
+  </si>
+  <si>
+    <t>sll $t1, $t1, 4</t>
+  </si>
+  <si>
+    <t>1100 111 000 000101</t>
+  </si>
+  <si>
+    <t>1000 001 001 000010</t>
+  </si>
+  <si>
+    <t>1110 100 011 100 000</t>
+  </si>
+  <si>
+    <t>1010 110 110 000100</t>
+  </si>
+  <si>
+    <t>1100 110 000 000100</t>
+  </si>
+  <si>
+    <t>1101 110 000 000001</t>
+  </si>
+  <si>
+    <t>1101 111 000 000000</t>
+  </si>
+  <si>
+    <t>1100 101 000 000001</t>
+  </si>
+  <si>
+    <t>0001 101 110 001100</t>
+  </si>
+  <si>
+    <t>0000 000 000 001011</t>
+  </si>
+  <si>
+    <t>sw $t0, Mem[$a0]</t>
+  </si>
+  <si>
+    <t>1101 001 000 000000</t>
+  </si>
+  <si>
+    <t>bgt $t0, 0, top</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +248,44 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -186,7 +332,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,9 +364,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -252,6 +399,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -427,156 +575,356 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="36.5703125" customWidth="1"/>
+    <col min="1" max="2" width="36.54296875" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="C33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>